<commit_message>
Create the lost page for users who are lost
</commit_message>
<xml_diff>
--- a/Documentation/Journaux_de_travail/Romain Lenoir/Journal_de_travail_I_Shoes.xlsx
+++ b/Documentation/Journaux_de_travail/Romain Lenoir/Journal_de_travail_I_Shoes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romai\Romain\GitHub DATA\I_Shoes\Documentation\Journaux_de_travail\Romain Lenoir\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romai\Romain\GitHub_DATA\I_Shoes\Documentation\Journaux_de_travail\Romain Lenoir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB32B046-A47D-4C67-B32B-6DF56228C810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC6C60E-6CFC-4D5D-9429-B9056669390D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8025" yWindow="1545" windowWidth="15510" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -719,7 +719,7 @@
   <dimension ref="A1:J1101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Create an argorithm for stock of articles
</commit_message>
<xml_diff>
--- a/Documentation/Journaux_de_travail/Romain Lenoir/Journal_de_travail_I_Shoes.xlsx
+++ b/Documentation/Journaux_de_travail/Romain Lenoir/Journal_de_travail_I_Shoes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romai\Romain\GitHub_DATA\I_Shoes\Documentation\Journaux_de_travail\Romain Lenoir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC6C60E-6CFC-4D5D-9429-B9056669390D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D82A1B-DCAD-4E34-89ED-EC4AF70FA51A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8025" yWindow="1545" windowWidth="15510" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="65">
   <si>
     <t>Date</t>
   </si>
@@ -195,9 +195,6 @@
     <t>Intègre les informations d'achat sous l'historique et optimise le model sur la gestion de panier</t>
   </si>
   <si>
-    <t>JSOn data</t>
-  </si>
-  <si>
     <t>Si l'utilisateur appuies sur le bouton de panier, la ligne spécifié dans la base de données du panier est détruit.</t>
   </si>
   <si>
@@ -217,6 +214,21 @@
   </si>
   <si>
     <t>https://stackoverflow.com/questions/11463581/how-to-use-unlink-function</t>
+  </si>
+  <si>
+    <t>Management</t>
+  </si>
+  <si>
+    <t>Longue recherche et création des divers articles du site</t>
+  </si>
+  <si>
+    <t>Gestion des stock</t>
+  </si>
+  <si>
+    <t>Pratique la gestion des stock de l'utilisateur</t>
+  </si>
+  <si>
+    <t>Json data</t>
   </si>
 </sst>
 </file>
@@ -718,8 +730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J1101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1443,16 +1455,16 @@
         <v>3.6805555555555536E-2</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G29" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="H29" s="21" t="s">
         <v>54</v>
-      </c>
-      <c r="H29" s="21" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1470,13 +1482,13 @@
         <v>2.4305555555555525E-2</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H30" s="13"/>
     </row>
@@ -1495,42 +1507,66 @@
         <v>5.555555555555558E-2</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F31" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G31" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="H31" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="H31" s="21" t="s">
+    </row>
+    <row r="32" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="7">
+        <v>45015</v>
+      </c>
+      <c r="B32" s="8">
+        <v>0.56597222222222221</v>
+      </c>
+      <c r="C32" s="8">
+        <v>0.70138888888888884</v>
+      </c>
+      <c r="D32" s="9">
+        <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
+        <v>0.13541666666666663</v>
+      </c>
+      <c r="E32" s="6" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="9">
-        <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>0</v>
-      </c>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
+      <c r="F32" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="H32" s="13"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
+    <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="7">
+        <v>45016</v>
+      </c>
+      <c r="B33" s="8">
+        <v>0.76388888888888884</v>
+      </c>
+      <c r="C33" s="8">
+        <v>0.78472222222222221</v>
+      </c>
       <c r="D33" s="9">
         <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>0</v>
-      </c>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="H33" s="13"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>